<commit_message>
style and update of the excel test to function mapping
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AD8B63-8CA1-4C06-95DC-9F8C8097119F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3626ED77-3910-4AEB-9F22-40AED60A8A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="139">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -191,9 +191,6 @@
     <t>__pipe_heat_to_discharge_path_constraints</t>
   </si>
   <si>
-    <t>__buffer_heat_to_discharge_path_constraints</t>
-  </si>
-  <si>
     <t>__heat_exchanger_heat_to_discharge_path_constraints</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
     <t>check for max discharge</t>
   </si>
   <si>
-    <t>x, missing heat loss var check, cost var check</t>
-  </si>
-  <si>
     <t>heat_pump_elec</t>
   </si>
   <si>
@@ -377,12 +371,6 @@
     <t>x, hardcoded pycml model</t>
   </si>
   <si>
-    <t>x, missing  assert statement</t>
-  </si>
-  <si>
-    <t>x, missing heat discharge check</t>
-  </si>
-  <si>
     <t>x, missing heat loss var check</t>
   </si>
   <si>
@@ -401,9 +389,6 @@
     <t>__flow_direction_path_constraints, use 3a</t>
   </si>
   <si>
-    <t>missing check, only heat loss is now checked</t>
-  </si>
-  <si>
     <t>use 1a</t>
   </si>
   <si>
@@ -425,26 +410,56 @@
     <t>add to sourc-sink test</t>
   </si>
   <si>
-    <t>x, hardcoded pycml</t>
-  </si>
-  <si>
-    <t>x, hardcoded pycml, missing  assert statement</t>
-  </si>
-  <si>
-    <t>hardcoded pycml model…, missing checks on this, now only history is checked which seems trivial and not needed</t>
-  </si>
-  <si>
     <t>no check of the actual head loss computation, could use 1a</t>
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>test_warmingup_unit_cases</t>
+  </si>
+  <si>
+    <t>test_1a</t>
+  </si>
+  <si>
+    <t>test_2a</t>
+  </si>
+  <si>
+    <t>test_3a</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>__storage_heat_to_discharge_path_constraints</t>
+  </si>
+  <si>
+    <t>__heat_loss_variable_constraints</t>
+  </si>
+  <si>
+    <t>test_topo_constraints</t>
+  </si>
+  <si>
+    <t>test_pipe_class_var</t>
+  </si>
+  <si>
+    <t>test_pipe_class_ordering_vars</t>
+  </si>
+  <si>
+    <t>test_head_loss_constraints</t>
+  </si>
+  <si>
+    <t>test_pump</t>
+  </si>
+  <si>
+    <t>test valves</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +492,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +543,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -548,6 +570,10 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -866,13 +892,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2DC776-9E13-4FEF-932A-CECB2CF372B3}">
-  <dimension ref="A1:BE52"/>
+  <dimension ref="A1:BF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,91 +907,92 @@
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -973,7 +1000,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -983,44 +1010,44 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB2" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AJ2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
-      <c r="AN2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AO2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
-      <c r="AR2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AS2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="AT2" s="2"/>
-      <c r="AU2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
@@ -1029,8 +1056,9 @@
       <c r="BB2" s="2"/>
       <c r="BC2" s="2"/>
       <c r="BD2" s="2"/>
-    </row>
-    <row r="3" spans="1:57" ht="288" x14ac:dyDescent="0.25">
+      <c r="BE2" s="2"/>
+    </row>
+    <row r="3" spans="1:58" ht="291.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1044,309 +1072,310 @@
         <v>46</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="W3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="W3" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="X3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="AA3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="AB3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AC3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AH3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI3" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AG3" s="7" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="AH3" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ3" s="9" t="s">
+      <c r="AK3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AK3" s="10" t="s">
+      <c r="AM3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AL3" s="10" t="s">
+      <c r="AN3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AO3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AP3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AO3" s="9" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AR3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AQ3" s="9" t="s">
+      <c r="AS3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AR3" s="10" t="s">
+      <c r="AT3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="AS3" s="9" t="s">
+      <c r="AU3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="AT3" s="10" t="s">
+      <c r="AV3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AU3" s="10" t="s">
+      <c r="AW3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AV3" s="9" t="s">
+      <c r="AX3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AW3" s="10" t="s">
+      <c r="AY3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AX3" s="9" t="s">
+      <c r="AZ3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AY3" s="10" t="s">
+      <c r="BA3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AZ3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="9" t="s">
+      <c r="BD3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BC3" s="9" t="s">
+      <c r="BE3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="BD3" s="9" t="s">
+      <c r="BF3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="BE3" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="AJ5" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK5" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="AL6" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="P7" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="Q7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AX7" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AY7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AW9" s="4"/>
-      <c r="AY9" s="4"/>
-    </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AW9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX9" s="4"/>
+      <c r="AZ9" s="4"/>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AW10" s="4"/>
-      <c r="AY10" s="4"/>
-    </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AW10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX10" s="4"/>
+      <c r="AZ10" s="4"/>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="BB13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BC13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="BE13" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="BD13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF13" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BB14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="BD14" s="5" t="s">
-        <v>64</v>
+      <c r="BC14" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="BE14" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AI16" s="5" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI17" s="5" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="AG18" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI18" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -1356,10 +1385,10 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
@@ -1367,15 +1396,15 @@
         <v>15</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AH22" s="5" t="s">
-        <v>112</v>
+      <c r="AI22" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
@@ -1383,15 +1412,15 @@
         <v>17</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
@@ -1434,243 +1463,348 @@
         <v>24</v>
       </c>
       <c r="U31" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AF32" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AG32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z33" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="5" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="AA33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB33" s="4"/>
       <c r="AC33" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD33" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AE33" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AZ35" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AR35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA35" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AZ36" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AR36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA36" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP40" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AQ40" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ41" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="AR41" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y43" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="Z43" s="4"/>
+    </row>
+    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AD44" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AE44" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="11"/>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AE48" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AF48" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>114</v>
+      <c r="H50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="S50" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y50" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>114</v>
+      <c r="H51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="S51" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y51" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L52" s="4" t="s">
-        <v>114</v>
+      <c r="H52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="S52" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y52" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54" t="s">
+        <v>130</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO54" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS54" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AV54" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z58" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z59" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:AF1"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AJ1:BD1"/>
+    <mergeCell ref="C1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:BE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
adding tests for heat node mixing
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3626ED77-3910-4AEB-9F22-40AED60A8A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C6C095-D359-434B-A2F0-25C3F66D961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="140">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>test valves</t>
+  </si>
+  <si>
+    <t>__node_discharge_mixing_path_constraints</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -574,6 +577,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -892,13 +898,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2DC776-9E13-4FEF-932A-CECB2CF372B3}">
-  <dimension ref="A1:BF63"/>
+  <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,148 +913,149 @@
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="C1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12" t="s">
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
         <v>117</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
-      <c r="AO2" s="2" t="s">
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
-      <c r="AS2" s="2" t="s">
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
-      <c r="AV2" s="2" t="s">
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AW2" s="2"/>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
       <c r="AZ2" s="2"/>
@@ -1057,600 +1064,601 @@
       <c r="BC2" s="2"/>
       <c r="BD2" s="2"/>
       <c r="BE2" s="2"/>
-    </row>
-    <row r="3" spans="1:58" ht="291.75" x14ac:dyDescent="0.25">
+      <c r="BF2" s="2"/>
+    </row>
+    <row r="3" spans="1:59" ht="291.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="W3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="X3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="AA3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AB3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AJ3" s="7" t="s">
+      <c r="AK3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="AK3" s="9" t="s">
+      <c r="AL3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AL3" s="10" t="s">
+      <c r="AM3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AN3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AO3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AO3" s="10" t="s">
+      <c r="AP3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AQ3" s="9" t="s">
+      <c r="AR3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AR3" s="9" t="s">
+      <c r="AS3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AS3" s="10" t="s">
+      <c r="AT3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AT3" s="9" t="s">
+      <c r="AU3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="AU3" s="10" t="s">
+      <c r="AV3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="AV3" s="10" t="s">
+      <c r="AW3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AW3" s="9" t="s">
+      <c r="AX3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AX3" s="10" t="s">
+      <c r="AY3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AY3" s="9" t="s">
+      <c r="AZ3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AZ3" s="10" t="s">
+      <c r="BA3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="BA3" s="9" t="s">
+      <c r="BB3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="9" t="s">
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="BD3" s="9" t="s">
+      <c r="BE3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BE3" s="9" t="s">
+      <c r="BF3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="BF3" s="9" t="s">
+      <c r="BG3" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="X4" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK5" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AL6" s="4" t="s">
+      <c r="AM6" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="Q7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AY7" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="R7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX9" s="4"/>
-      <c r="AZ9" s="4"/>
-    </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="S9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY9" s="4"/>
+      <c r="BA9" s="4"/>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="R10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX10" s="4"/>
-      <c r="AZ10" s="4"/>
-    </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="S10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY10" s="4"/>
+      <c r="BA10" s="4"/>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC13" s="5" t="s">
+      <c r="W13" s="5" t="s">
         <v>63</v>
       </c>
       <c r="BD13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="BF13" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="BE13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG13" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BC14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE14" s="5" t="s">
+      <c r="BD14" s="5" t="s">
         <v>63</v>
       </c>
       <c r="BF14" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="BG14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AI22" s="5" t="s">
+      <c r="AJ22" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="11"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U31" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="V31" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AG32" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AH32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="U33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC33" s="4"/>
       <c r="AD33" s="5" t="s">
         <v>63</v>
       </c>
       <c r="AE33" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AF33" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA35" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="M35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB35" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA36" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="M36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB36" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="L37" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="M37" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L40" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ40" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="M40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR40" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR41" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="M41" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS41" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O43" s="4" t="s">
+      <c r="P43" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="U43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z43" s="4"/>
-    </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="V43" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA43" s="4"/>
+    </row>
+    <row r="44" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AE44" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AF44" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="11"/>
     </row>
-    <row r="46" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AF48" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AG48" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I50" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="S50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y50" s="4" t="s">
+      <c r="K50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T50" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z50" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H51" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I51" s="5" t="s">
         <v>63</v>
       </c>
@@ -1660,20 +1668,20 @@
       <c r="K51" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="S51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y51" s="4" t="s">
+      <c r="L51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z51" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H52" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I52" s="5" t="s">
         <v>63</v>
       </c>
@@ -1686,71 +1694,74 @@
       <c r="L52" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="S52" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y52" s="4" t="s">
+      <c r="M52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z52" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54" t="s">
         <v>130</v>
       </c>
-      <c r="F54" t="s">
+      <c r="I54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO54" s="4" t="s">
+      <c r="AT54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AS54" s="4" t="s">
+      <c r="AW54" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AV54" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I55" s="5" t="s">
         <v>63</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="K55" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>130</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I56" s="5" t="s">
         <v>63</v>
       </c>
@@ -1760,51 +1771,54 @@
       <c r="K56" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="L56" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>134</v>
       </c>
-      <c r="Y58" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="Z58" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AA58" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>135</v>
       </c>
-      <c r="Z59" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AA59" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:AG1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK1:BE1"/>
+    <mergeCell ref="C1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:BF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added assert statement for max discharge under pipe class optimization
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C6C095-D359-434B-A2F0-25C3F66D961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E49BD80-482F-4B81-BE8D-65459DC754C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="138">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -353,9 +353,6 @@
     <t>head_loss_mixin</t>
   </si>
   <si>
-    <t>check for max discharge</t>
-  </si>
-  <si>
     <t>heat_pump_elec</t>
   </si>
   <si>
@@ -381,9 +378,6 @@
   </si>
   <si>
     <t>missing simple separate check, use 1a</t>
-  </si>
-  <si>
-    <t>__node_discharge_mixing_path_constraints, use 1a</t>
   </si>
   <si>
     <t>__flow_direction_path_constraints, use 3a</t>
@@ -904,7 +898,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
+      <selection pane="bottomRight" activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,28 +973,28 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1008,7 +1002,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1018,15 +1012,15 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Z2" s="3"/>
       <c r="AA2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -1036,25 +1030,25 @@
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
@@ -1077,16 +1071,13 @@
         <v>45</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>47</v>
@@ -1101,7 +1092,7 @@
         <v>50</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>51</v>
@@ -1112,7 +1103,7 @@
       <c r="O3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>54</v>
       </c>
       <c r="Q3" s="9" t="s">
@@ -1143,7 +1134,7 @@
         <v>92</v>
       </c>
       <c r="Z3" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>93</v>
@@ -1227,7 +1218,7 @@
         <v>82</v>
       </c>
       <c r="BB3" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BC3" s="1"/>
       <c r="BD3" s="9" t="s">
@@ -1267,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="AM6" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
@@ -1296,7 +1287,7 @@
         <v>64</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>63</v>
@@ -1313,7 +1304,7 @@
         <v>65</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>63</v>
@@ -1399,7 +1390,7 @@
         <v>89</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
@@ -1415,7 +1406,7 @@
         <v>16</v>
       </c>
       <c r="AJ22" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
@@ -1423,7 +1414,7 @@
         <v>17</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
@@ -1431,7 +1422,7 @@
         <v>91</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
@@ -1541,7 +1532,7 @@
     </row>
     <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>63</v>
@@ -1588,8 +1579,8 @@
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="P43" s="4" t="s">
-        <v>105</v>
+      <c r="P43" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="V43" s="5" t="s">
         <v>63</v>
@@ -1652,7 +1643,7 @@
         <v>63</v>
       </c>
       <c r="Z50" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
@@ -1675,7 +1666,7 @@
         <v>63</v>
       </c>
       <c r="Z51" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.25">
@@ -1701,17 +1692,17 @@
         <v>63</v>
       </c>
       <c r="Z52" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>63</v>
@@ -1719,9 +1710,6 @@
       <c r="D54" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G54" t="s">
-        <v>130</v>
-      </c>
       <c r="I54" s="5" t="s">
         <v>63</v>
       </c>
@@ -1732,18 +1720,18 @@
         <v>63</v>
       </c>
       <c r="AP54" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AT54" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AW54" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>63</v>
@@ -1757,10 +1745,10 @@
     </row>
     <row r="56" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F56" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>63</v>
@@ -1777,12 +1765,12 @@
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Z58" s="5" t="s">
         <v>63</v>
@@ -1793,7 +1781,7 @@
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AA59" s="5" t="s">
         <v>63</v>
@@ -1801,17 +1789,17 @@
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added heat loss check under varying network temperature
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E49BD80-482F-4B81-BE8D-65459DC754C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF51C24F-38F3-4A9E-9E27-FE2BEF2B7A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="137">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -366,9 +366,6 @@
   </si>
   <si>
     <t>x, hardcoded pycml model</t>
-  </si>
-  <si>
-    <t>x, missing heat loss var check</t>
   </si>
   <si>
     <t>missing simple separate check</t>
@@ -898,7 +895,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R39" sqref="R39"/>
+      <selection pane="bottomRight" activeCell="Z35" sqref="Z35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,28 +970,28 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1002,7 +999,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1012,15 +1009,15 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z2" s="3"/>
       <c r="AA2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -1030,25 +1027,25 @@
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
@@ -1071,13 +1068,13 @@
         <v>45</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>47</v>
@@ -1092,7 +1089,7 @@
         <v>50</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>51</v>
@@ -1133,8 +1130,8 @@
       <c r="Y3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Z3" s="7" t="s">
-        <v>130</v>
+      <c r="Z3" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>93</v>
@@ -1258,7 +1255,7 @@
         <v>3</v>
       </c>
       <c r="AM6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
@@ -1287,7 +1284,7 @@
         <v>64</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>63</v>
@@ -1304,7 +1301,7 @@
         <v>65</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>63</v>
@@ -1576,7 +1573,7 @@
       </c>
     </row>
     <row r="43" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>31</v>
       </c>
       <c r="P43" s="5" t="s">
@@ -1585,7 +1582,9 @@
       <c r="V43" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AA43" s="4"/>
+      <c r="AA43" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="44" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -1627,7 +1626,7 @@
       </c>
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>42</v>
       </c>
       <c r="I50" s="5" t="s">
@@ -1642,12 +1641,12 @@
       <c r="T50" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Z50" s="4" t="s">
-        <v>110</v>
+      <c r="Z50" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I51" s="5" t="s">
@@ -1665,12 +1664,12 @@
       <c r="T51" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Z51" s="4" t="s">
-        <v>110</v>
+      <c r="Z51" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>44</v>
       </c>
       <c r="I52" s="5" t="s">
@@ -1691,18 +1690,18 @@
       <c r="T52" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Z52" s="4" t="s">
-        <v>110</v>
+      <c r="Z52" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>63</v>
@@ -1720,18 +1719,18 @@
         <v>63</v>
       </c>
       <c r="AP54" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AT54" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AW54" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>63</v>
@@ -1745,10 +1744,10 @@
     </row>
     <row r="56" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F56" t="s">
         <v>127</v>
-      </c>
-      <c r="F56" t="s">
-        <v>128</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>63</v>
@@ -1765,12 +1764,12 @@
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z58" s="5" t="s">
         <v>63</v>
@@ -1781,7 +1780,7 @@
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA59" s="5" t="s">
         <v>63</v>
@@ -1789,17 +1788,17 @@
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests for node, demand and source
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF51C24F-38F3-4A9E-9E27-FE2BEF2B7A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544CF0A8-09DD-412B-9744-A7378214038F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="137">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -892,10 +892,10 @@
   <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="N16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z35" sqref="Z35"/>
+      <selection pane="bottomRight" activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
       <c r="AB3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AC3" s="8" t="s">
         <v>95</v>
       </c>
       <c r="AD3" s="8" t="s">
@@ -1157,7 +1157,7 @@
       <c r="AH3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AI3" s="7" t="s">
+      <c r="AI3" s="8" t="s">
         <v>102</v>
       </c>
       <c r="AJ3" s="8" t="s">
@@ -1178,7 +1178,7 @@
       <c r="AO3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AP3" s="10" t="s">
+      <c r="AP3" s="9" t="s">
         <v>71</v>
       </c>
       <c r="AQ3" s="9" t="s">
@@ -1190,7 +1190,7 @@
       <c r="AS3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AT3" s="10" t="s">
+      <c r="AT3" s="9" t="s">
         <v>75</v>
       </c>
       <c r="AU3" s="9" t="s">
@@ -1199,7 +1199,7 @@
       <c r="AV3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="AW3" s="10" t="s">
+      <c r="AW3" s="9" t="s">
         <v>78</v>
       </c>
       <c r="AX3" s="9" t="s">
@@ -1483,7 +1483,9 @@
       <c r="AB33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AC33" s="4"/>
+      <c r="AC33" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="AD33" s="5" t="s">
         <v>63</v>
       </c>
@@ -1718,14 +1720,17 @@
       <c r="K54" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AP54" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT54" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW54" s="4" t="s">
-        <v>127</v>
+      <c r="AI54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW54" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added test for electricity source and demand component
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544CF0A8-09DD-412B-9744-A7378214038F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC8D000-47D5-4808-9B49-15E840164E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="137">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -892,10 +892,10 @@
   <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AP3" sqref="AP3"/>
+      <selection pane="bottomRight" activeCell="AY29" sqref="AY29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,13 +1205,13 @@
       <c r="AX3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AY3" s="10" t="s">
+      <c r="AY3" s="9" t="s">
         <v>80</v>
       </c>
       <c r="AZ3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="BA3" s="10" t="s">
+      <c r="BA3" s="9" t="s">
         <v>82</v>
       </c>
       <c r="BB3" s="9" t="s">
@@ -1292,8 +1292,12 @@
       <c r="AX9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AY9" s="4"/>
-      <c r="BA9" s="4"/>
+      <c r="AY9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA9" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1309,8 +1313,6 @@
       <c r="AX10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AY10" s="4"/>
-      <c r="BA10" s="4"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">

</xml_diff>

<commit_message>
tests for electricity demands
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC8D000-47D5-4808-9B49-15E840164E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0844D521-1CA9-4307-9B02-9B7E84725898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -892,10 +892,10 @@
   <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY29" sqref="AY29"/>
+      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>26</v>
       </c>
       <c r="U33" s="5" t="s">
@@ -1704,7 +1704,7 @@
       </c>
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>124</v>
       </c>
       <c r="C54" s="5" t="s">

</xml_diff>

<commit_message>
updated test matrix excel
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0844D521-1CA9-4307-9B02-9B7E84725898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F3295C-A0E9-4E6D-A21B-586328B670C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -892,10 +892,10 @@
   <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,18 +1273,18 @@
       </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>127</v>
+      <c r="Q9" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>63</v>
@@ -1300,12 +1300,12 @@
       </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>127</v>
+      <c r="Q10" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
updated matrix and removed old buffer test
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F3295C-A0E9-4E6D-A21B-586328B670C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDED500-E886-4E23-9C82-F1275353BD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="134">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Test_ates</t>
   </si>
   <si>
-    <t>test_buffer</t>
-  </si>
-  <si>
     <t>test_electric_bus</t>
   </si>
   <si>
@@ -386,9 +383,6 @@
     <t>use 1a also in standard non temperature varying case</t>
   </si>
   <si>
-    <t>use 3a to check</t>
-  </si>
-  <si>
     <t>add to diameter sizing test</t>
   </si>
   <si>
@@ -417,9 +411,6 @@
   </si>
   <si>
     <t>test_3a</t>
-  </si>
-  <si>
-    <t>missing</t>
   </si>
   <si>
     <t>__storage_heat_to_discharge_path_constraints</t>
@@ -892,10 +883,10 @@
   <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="AM6" sqref="AM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +897,7 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="C1" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
@@ -940,12 +931,12 @@
       <c r="AG1" s="14"/>
       <c r="AH1" s="14"/>
       <c r="AI1" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AJ1" s="14"/>
       <c r="AK1" s="14"/>
       <c r="AL1" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AM1" s="14"/>
       <c r="AN1" s="14"/>
@@ -970,28 +961,28 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -999,7 +990,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1009,15 +1000,15 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z2" s="3"/>
       <c r="AA2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -1027,25 +1018,25 @@
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
@@ -1059,176 +1050,176 @@
     </row>
     <row r="3" spans="1:59" ht="291.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="W3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="X3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="X3" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="Y3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AB3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AC3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AK3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AJ3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK3" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="AL3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AN3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AO3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AO3" s="10" t="s">
+      <c r="AP3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="AQ3" s="9" t="s">
+      <c r="AR3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AR3" s="9" t="s">
+      <c r="AS3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AS3" s="9" t="s">
+      <c r="AT3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AT3" s="9" t="s">
+      <c r="AU3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="AU3" s="9" t="s">
+      <c r="AV3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AV3" s="10" t="s">
+      <c r="AW3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="AW3" s="9" t="s">
+      <c r="AX3" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="AX3" s="9" t="s">
+      <c r="AY3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AY3" s="9" t="s">
+      <c r="AZ3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AZ3" s="9" t="s">
+      <c r="BA3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="BA3" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="BB3" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BC3" s="1"/>
       <c r="BD3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="BE3" s="9" t="s">
+      <c r="BF3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BF3" s="9" t="s">
+      <c r="BG3" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="BG3" s="9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
@@ -1236,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
@@ -1244,568 +1235,563 @@
         <v>2</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AZ7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AX9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AY9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BA9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AX10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BD13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BE13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BG13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BD14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BF14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BG14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ22" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="11"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V31" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH32" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AF33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS35" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB35" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS36" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BB36" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AR40" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS41" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V43" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA43" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AF44" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="11"/>
     </row>
     <row r="46" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AG48" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AP54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AT54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AW54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F56" t="s">
-        <v>127</v>
+      <c r="B56" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="AM56" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z58" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA58" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AA59" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using a simple esdl based test for test_heat.py
</commit_message>
<xml_diff>
--- a/tests/Functionality_test_matrix.xlsx
+++ b/tests/Functionality_test_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojerj\Documents\Git\NWN\rtc-tools-heat-network\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDED500-E886-4E23-9C82-F1275353BD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45EC185-B338-4B1F-BD0A-7E9E1D62E35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DAAF6E-EE2D-4FFD-A3BD-71B71243616C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="131">
   <si>
     <t>test function/connstraint function</t>
   </si>
@@ -305,9 +305,6 @@
     <t>test_heat_loss</t>
   </si>
   <si>
-    <t>missing assert statement</t>
-  </si>
-  <si>
     <t>test_disconnected_network_pipe_no_heat_loss</t>
   </si>
   <si>
@@ -354,12 +351,6 @@
   </si>
   <si>
     <t>test_heat_pump_elec_min_elec</t>
-  </si>
-  <si>
-    <t>x, Hardcoded pycml model</t>
-  </si>
-  <si>
-    <t>x, hardcoded pycml model, indexing in last assert statement is weird</t>
   </si>
   <si>
     <t>x, hardcoded pycml model</t>
@@ -444,7 +435,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,13 +458,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -489,7 +473,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,11 +490,6 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -521,14 +500,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -539,9 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -554,20 +530,19 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -883,10 +858,10 @@
   <dimension ref="A1:BG63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AM6" sqref="AM6"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,93 +871,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
-      <c r="AL1" s="14" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="D2" s="10"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -990,7 +965,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1000,15 +975,15 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z2" s="3"/>
       <c r="AA2" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -1018,25 +993,25 @@
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
@@ -1048,317 +1023,317 @@
       <c r="BE2" s="2"/>
       <c r="BF2" s="2"/>
     </row>
-    <row r="3" spans="1:59" ht="291.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="288" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="L3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="V3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="X3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Y3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA3" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="Z3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AB3" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AC3" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AF3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AI3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AK3" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AJ3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="AL3" s="9" t="s">
+      <c r="AL3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AM3" s="9" t="s">
+      <c r="AM3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AN3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AO3" s="10" t="s">
+      <c r="AO3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AP3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AQ3" s="9" t="s">
+      <c r="AQ3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AR3" s="9" t="s">
+      <c r="AR3" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AS3" s="9" t="s">
+      <c r="AS3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AT3" s="9" t="s">
+      <c r="AT3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AU3" s="9" t="s">
+      <c r="AU3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="AV3" s="10" t="s">
+      <c r="AV3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="AW3" s="9" t="s">
+      <c r="AW3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AX3" s="9" t="s">
+      <c r="AX3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="AY3" s="9" t="s">
+      <c r="AY3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AZ3" s="9" t="s">
+      <c r="AZ3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="BA3" s="9" t="s">
+      <c r="BA3" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="BB3" s="9" t="s">
-        <v>104</v>
+      <c r="BB3" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="BC3" s="1"/>
-      <c r="BD3" s="9" t="s">
+      <c r="BD3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="BE3" s="9" t="s">
+      <c r="BE3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="BF3" s="9" t="s">
+      <c r="BF3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="BG3" s="9" t="s">
+      <c r="BG3" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL5" s="5" t="s">
+      <c r="H5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL5" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AZ7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ7" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Q9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AY9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BA9" s="5" t="s">
+      <c r="Q9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BA9" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="Q10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AX10" s="5" t="s">
+      <c r="Q10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX10" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BD13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BE13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BG13" s="5" t="s">
+      <c r="W13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG13" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="BD14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BF14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BG14" s="5" t="s">
+      <c r="BD14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG14" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1368,11 +1343,11 @@
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>106</v>
+      <c r="E20" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
@@ -1380,104 +1355,107 @@
         <v>14</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ22" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ22" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>107</v>
+      <c r="F24" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="F25" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="V31" s="5" t="s">
+      <c r="V31" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AH32" s="5" t="s">
+      <c r="AH32" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF33" s="5" t="s">
+      <c r="U33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF33" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1487,43 +1465,43 @@
       </c>
     </row>
     <row r="35" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BB35" s="5" t="s">
+      <c r="M35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB35" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="BB36" s="5" t="s">
+      <c r="M36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB36" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="M37" s="5" t="s">
+      <c r="B37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M37" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1533,24 +1511,24 @@
       </c>
     </row>
     <row r="40" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AR40" s="5" t="s">
+      <c r="M40" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR40" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M41" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS41" s="5" t="s">
+      <c r="M41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS41" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1560,50 +1538,50 @@
       </c>
     </row>
     <row r="43" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="P43" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="V43" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA43" s="5" t="s">
+      <c r="P43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA43" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AF44" s="5" t="s">
+      <c r="AF44" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="11"/>
+      <c r="B45" s="9"/>
     </row>
     <row r="46" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AG48" s="5" t="s">
+      <c r="AG48" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1613,185 +1591,185 @@
       </c>
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I50" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T50" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z50" s="5" t="s">
+      <c r="I50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z50" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K51" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L51" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T51" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z51" s="5" t="s">
+      <c r="I51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z51" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z52" s="5" t="s">
+      <c r="I52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z52" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT54" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW54" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AW54" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K55" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM56" s="5" t="s">
+      <c r="F56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM56" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z58" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA58" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA59" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="Z58" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA58" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    </row>
+    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="AA59" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>